<commit_message>
Added new samples from different runs for test
Changed the location of the fastq files from the repo to the file share
</commit_message>
<xml_diff>
--- a/test/COVID_Dragen_bs/metadata/extra_metadata/test_EpiSheet_filtered.xlsx
+++ b/test/COVID_Dragen_bs/metadata/extra_metadata/test_EpiSheet_filtered.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://phila-my.sharepoint.com/personal/vincent_tu_phila_gov/Documents/RmdTemplates/test/COVID_Dragen_bs/metadata/extra_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="11_E24288542448A208B4ECAC86FC1270E9D9049F5B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54B2CD14-145F-47C4-92E3-BFA22D8C95E2}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="11_E24288542448A208B4ECAC86FC1270E9D9049F5B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D92723D-36B2-4EA7-AC8A-1CA3799E243E}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="49">
   <si>
     <t>SPECIMEN_DATE</t>
   </si>
@@ -150,6 +150,24 @@
   </si>
   <si>
     <t>No variant calls</t>
+  </si>
+  <si>
+    <t>Arya Stark</t>
+  </si>
+  <si>
+    <t>Test-Sample4</t>
+  </si>
+  <si>
+    <t>BQ.1.1</t>
+  </si>
+  <si>
+    <t>Test-Sample5</t>
+  </si>
+  <si>
+    <t>XBB.1.5.1</t>
+  </si>
+  <si>
+    <t>Missandei</t>
   </si>
 </sst>
 </file>
@@ -224,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -256,6 +274,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -559,7 +578,7 @@
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1:T3"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,10 +753,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,6 +854,67 @@
         <v>42</v>
       </c>
     </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
+        <v>44747</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3">
+        <v>20.5</v>
+      </c>
+      <c r="H3">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>44744</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4">
+        <v>26.5</v>
+      </c>
+      <c r="H4">
+        <v>25</v>
+      </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O4" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>